<commit_message>
Added Effective Date code
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Leave_Type_Repository.xlsx
+++ b/src/main/resources/TestData/Leave_Type_Repository.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LeaveType1_Scenarios" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7643" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7627" uniqueCount="738">
   <si>
     <t xml:space="preserve">Test Case</t>
   </si>
@@ -3250,30 +3250,6 @@
   </si>
   <si>
     <t xml:space="preserve">Current Date Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5ab0c55952fe8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-03-20T13:54:59.316</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5ab0c592ea4fe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-03-20T13:55:57.071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5ab0cbe394932</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-03-20T14:22:53.672</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5ab0cc37dca19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-03-20T14:24:17.845</t>
   </si>
   <si>
     <t xml:space="preserve">Leave Type 1</t>
@@ -4153,18 +4129,18 @@
   <dimension ref="A1:U209"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="B2:B3 E3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17771,18 +17747,18 @@
   <dimension ref="A1:U209"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="1" sqref="B2:B3 D24"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31386,19 +31362,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B3"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31413,34 +31389,6 @@
       </c>
       <c r="D1" s="6" t="s">
         <v>652</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>653</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>655</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -31459,19 +31407,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31486,34 +31434,6 @@
       </c>
       <c r="D1" s="6" t="s">
         <v>652</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>463</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>657</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>464</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>659</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>660</v>
       </c>
     </row>
   </sheetData>
@@ -31534,22 +31454,22 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31587,428 +31507,428 @@
   <dimension ref="A1:A83"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B2:B3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="91.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>